<commit_message>
chore: Add 12/23 paycheck
</commit_message>
<xml_diff>
--- a/paycheck_info.xlsx
+++ b/paycheck_info.xlsx
@@ -65,9 +65,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
-    <numFmt numFmtId="59" formatCode="m/d/yyyy"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -129,7 +128,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -146,12 +145,6 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="59" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -1687,13 +1680,13 @@
       <c r="D9" s="5">
         <v>931.92</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="4">
         <v>44881</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="4">
         <v>44895</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="4">
         <v>44903</v>
       </c>
       <c r="H9" s="5">
@@ -1726,22 +1719,55 @@
       </c>
     </row>
     <row r="10" ht="13.55" customHeight="1">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="7"/>
+      <c r="A10" s="5">
+        <v>291.81</v>
+      </c>
+      <c r="B10" s="5">
+        <v>1734.09</v>
+      </c>
+      <c r="C10" s="3">
+        <v>912.9</v>
+      </c>
+      <c r="D10" s="5">
+        <v>621.09</v>
+      </c>
+      <c r="E10" s="4">
+        <v>44896</v>
+      </c>
+      <c r="F10" s="4">
+        <v>44910</v>
+      </c>
+      <c r="G10" s="4">
+        <v>44918</v>
+      </c>
+      <c r="H10" s="5">
+        <v>60.51</v>
+      </c>
+      <c r="I10" s="5">
+        <v>0.7</v>
+      </c>
+      <c r="J10" s="5">
+        <v>59.81</v>
+      </c>
+      <c r="K10" s="5">
+        <v>29.11</v>
+      </c>
+      <c r="L10" s="5">
+        <v>38.38</v>
+      </c>
+      <c r="M10" s="5">
+        <v>108.49</v>
+      </c>
+      <c r="N10" s="3">
+        <v>281</v>
+      </c>
+      <c r="O10" s="5">
+        <v>164.11</v>
+      </c>
+      <c r="P10" s="3">
+        <f>D10/(B10+C10)</f>
+        <v>0.234640100642617</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>